<commit_message>
final review RT andres
</commit_message>
<xml_diff>
--- a/RT/docs/acronyms.xlsx
+++ b/RT/docs/acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositaries\1.work\IAEA\RT\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9852492F-1735-4429-9EAA-435657E491AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08C7C8A-DBDD-46F6-8BAF-BDA747A1E33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA01B3EA-B5FB-4AC1-B03B-C97842D39369}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,43 +517,43 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -566,50 +566,50 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
+      <c r="A11" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -622,7 +622,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B13">
-    <sortCondition ref="B2:B13"/>
+    <sortCondition ref="A2:A13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>